<commit_message>
jam file hyperlink implement
</commit_message>
<xml_diff>
--- a/JAM editor요구사항.xlsx
+++ b/JAM editor요구사항.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://o365uos-my.sharepoint.com/personal/2016440063_office_uos_ac_kr/Documents/JAVA/kr.ac.uos.ai.editor.jamEditor/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5734DD0-2FF4-40B2-B1BE-1BDDE0E42430}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="31" documentId="13_ncr:1_{E5734DD0-2FF4-40B2-B1BE-1BDDE0E42430}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B474D7ED-31C3-426C-9A92-3EE7028D57EF}"/>
   <bookViews>
-    <workbookView xWindow="-50" yWindow="870" windowWidth="33430" windowHeight="17900" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="75">
   <si>
     <t>유즈케이스</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -112,10 +112,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>world model에 접근하는 명령을 coloring 할 수 있어야 한다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>perform, achieve, maintain, conclude 단어를 coloring 할 수 있어야 한다.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -153,9 +149,6 @@
   </si>
   <si>
     <t>id, name, precondition, context, body, utility 단어를 coloring 할 수 있어야 한다.</t>
-  </si>
-  <si>
-    <t>fact, retrieve, match, update 단어를 coloring 할 수 있어야 한다.</t>
   </si>
   <si>
     <t>prefixes 안의 prefix된 단어들을 coloring 할 수 있어야 한다.</t>
@@ -303,15 +296,35 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>assert, retract도 해야 함</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>plan achieve someGoal($arg1, $arg2){}</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>위와 같이 선언되어있을 경우 achieve는 goal action, someGoal은 relation or goal이라 부름 achieve someGoal은 뭐라 불러야 하나..</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fact, retrieve, match, update, retract, assert 단어를 coloring 할 수 있어야 한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>world model action을 coloring 할 수 있어야 한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>x</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">body:가 아닌 빈 공간에서 자동 완성 커맨드(Ctrl + space)사용 시 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>body:가 goal action 이후 자동 완성 커맨드(Ctrl + space)사용 시</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>없애도 될 듯</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -700,8 +713,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1ABE5394-59B4-47FD-BA35-BF7A817F817E}">
   <dimension ref="B1:I48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -729,16 +742,16 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>5</v>
       </c>
       <c r="I1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2" spans="2:9" x14ac:dyDescent="0.45">
@@ -749,7 +762,7 @@
         <v>20</v>
       </c>
       <c r="E2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F2">
         <v>5</v>
@@ -758,15 +771,15 @@
         <v>1</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.45">
       <c r="D3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F3">
         <v>5</v>
@@ -775,15 +788,15 @@
         <v>1</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.45">
       <c r="D4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F4">
         <v>5</v>
@@ -792,15 +805,15 @@
         <v>1</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.45">
       <c r="D5" t="s">
-        <v>21</v>
+        <v>70</v>
       </c>
       <c r="E5" t="s">
-        <v>32</v>
+        <v>69</v>
       </c>
       <c r="F5">
         <v>5</v>
@@ -809,34 +822,38 @@
         <v>1</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.45">
       <c r="D6" t="s">
-        <v>23</v>
+        <v>56</v>
       </c>
       <c r="E6" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="F6">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G6">
         <v>1</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.45">
       <c r="D7" t="s">
-        <v>58</v>
+        <v>22</v>
       </c>
       <c r="E7" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.45">
-      <c r="D8" t="s">
-        <v>69</v>
+        <v>31</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.45">
@@ -844,24 +861,30 @@
         <v>13</v>
       </c>
       <c r="D10" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E10" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G10">
         <v>3</v>
       </c>
+      <c r="H10" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="I10" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.45">
       <c r="D11" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E11" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F11">
         <v>2</v>
@@ -869,13 +892,19 @@
       <c r="G11">
         <v>3</v>
       </c>
+      <c r="H11" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="I11" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.45">
       <c r="D12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E12" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F12">
         <v>3</v>
@@ -883,19 +912,28 @@
       <c r="G12">
         <v>3</v>
       </c>
+      <c r="H12" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="I12" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.45">
       <c r="D13" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E13" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F13">
         <v>1</v>
       </c>
       <c r="G13">
         <v>2</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.45">
@@ -903,55 +941,55 @@
         <v>14</v>
       </c>
       <c r="D15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E15" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F15">
         <v>1</v>
       </c>
       <c r="G15" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.45">
       <c r="D16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E16" t="s">
+        <v>42</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="G16" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" spans="3:8" x14ac:dyDescent="0.45">
+      <c r="D17" t="s">
+        <v>53</v>
+      </c>
+      <c r="E17" t="s">
         <v>44</v>
       </c>
-      <c r="F16">
-        <v>1</v>
-      </c>
-      <c r="G16" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="17" spans="3:7" x14ac:dyDescent="0.45">
-      <c r="D17" t="s">
-        <v>55</v>
-      </c>
-      <c r="E17" t="s">
-        <v>46</v>
-      </c>
       <c r="F17">
         <v>1</v>
       </c>
       <c r="G17" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="19" spans="3:7" x14ac:dyDescent="0.45">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="3:8" x14ac:dyDescent="0.45">
       <c r="C19" t="s">
         <v>15</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E19" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F19">
         <v>5</v>
@@ -959,68 +997,86 @@
       <c r="G19">
         <v>4</v>
       </c>
-    </row>
-    <row r="20" spans="3:7" x14ac:dyDescent="0.45">
+      <c r="H19" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="20" spans="3:8" x14ac:dyDescent="0.45">
       <c r="D20" s="3"/>
       <c r="E20" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F20">
         <v>5</v>
       </c>
-    </row>
-    <row r="21" spans="3:7" x14ac:dyDescent="0.45">
+      <c r="H20" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="21" spans="3:8" x14ac:dyDescent="0.45">
       <c r="D21" s="3"/>
       <c r="E21" t="s">
+        <v>60</v>
+      </c>
+      <c r="F21">
+        <v>5</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="22" spans="3:8" ht="34" x14ac:dyDescent="0.45">
+      <c r="D22" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E22" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="F21">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="22" spans="3:7" ht="34" x14ac:dyDescent="0.45">
-      <c r="D22" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>64</v>
-      </c>
       <c r="F22">
         <v>5</v>
       </c>
-    </row>
-    <row r="23" spans="3:7" x14ac:dyDescent="0.45">
+      <c r="H22" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="23" spans="3:8" x14ac:dyDescent="0.45">
       <c r="D23" s="3"/>
       <c r="E23" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F23">
         <v>5</v>
       </c>
-    </row>
-    <row r="27" spans="3:7" x14ac:dyDescent="0.45">
+      <c r="H23" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="27" spans="3:8" x14ac:dyDescent="0.45">
       <c r="C27" t="s">
         <v>16</v>
       </c>
       <c r="D27" t="s">
+        <v>27</v>
+      </c>
+      <c r="E27" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E27" s="1" t="s">
-        <v>29</v>
-      </c>
       <c r="F27">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G27">
         <v>2</v>
       </c>
-    </row>
-    <row r="29" spans="3:7" x14ac:dyDescent="0.45">
+      <c r="H27" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="29" spans="3:8" x14ac:dyDescent="0.45">
       <c r="C29" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D29" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F29">
         <v>5</v>
@@ -1028,16 +1084,22 @@
       <c r="G29">
         <v>3</v>
       </c>
-    </row>
-    <row r="30" spans="3:7" x14ac:dyDescent="0.45">
+      <c r="H29" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="30" spans="3:8" x14ac:dyDescent="0.45">
       <c r="D30" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F30">
         <v>5</v>
       </c>
       <c r="G30">
         <v>3</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="34" spans="3:9" x14ac:dyDescent="0.45">
@@ -1045,10 +1107,10 @@
         <v>17</v>
       </c>
       <c r="D34" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E34" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F34">
         <v>0</v>
@@ -1059,16 +1121,16 @@
         <v>18</v>
       </c>
       <c r="D35" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E35" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F35">
         <v>0</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="36" spans="3:9" x14ac:dyDescent="0.45">
@@ -1076,10 +1138,10 @@
         <v>19</v>
       </c>
       <c r="D36" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E36" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F36">
         <v>0</v>
@@ -1087,15 +1149,15 @@
     </row>
     <row r="47" spans="3:9" x14ac:dyDescent="0.45">
       <c r="C47" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D47" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="48" spans="3:9" ht="34" x14ac:dyDescent="0.45">
       <c r="D48" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
FACTS에 있는 fact action relation에 추가, syntax error marker, plan id error marker 변경
</commit_message>
<xml_diff>
--- a/JAM editor요구사항.xlsx
+++ b/JAM editor요구사항.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://o365uos-my.sharepoint.com/personal/2016440063_office_uos_ac_kr/Documents/JAVA/kr.ac.uos.ai.editor.jamEditor/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="31" documentId="13_ncr:1_{E5734DD0-2FF4-40B2-B1BE-1BDDE0E42430}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B474D7ED-31C3-426C-9A92-3EE7028D57EF}"/>
+  <xr:revisionPtr revIDLastSave="54" documentId="13_ncr:1_{E5734DD0-2FF4-40B2-B1BE-1BDDE0E42430}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0E512EBB-69B6-4F54-9E03-7D035E5785C2}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="77">
   <si>
     <t>유즈케이스</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -325,6 +325,14 @@
   </si>
   <si>
     <t>없애도 될 듯</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>id가 없는 플랜을 찾을 수 있어야 한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>id가 중복된 플랜을 찾을 수 있어야 한다.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -368,13 +376,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -394,6 +405,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -714,7 +729,7 @@
   <dimension ref="B1:I48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -723,7 +738,7 @@
     <col min="3" max="3" width="20.58203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="69.08203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="97.83203125" customWidth="1"/>
-    <col min="6" max="7" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="10.6640625" style="3" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="4.83203125" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="66.58203125" customWidth="1"/>
   </cols>
@@ -741,10 +756,10 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="3" t="s">
         <v>40</v>
       </c>
       <c r="H1" s="2" t="s">
@@ -764,10 +779,10 @@
       <c r="E2" t="s">
         <v>21</v>
       </c>
-      <c r="F2">
-        <v>5</v>
-      </c>
-      <c r="G2">
+      <c r="F2" s="3">
+        <v>5</v>
+      </c>
+      <c r="G2" s="3">
         <v>1</v>
       </c>
       <c r="H2" s="2" t="s">
@@ -781,10 +796,10 @@
       <c r="E3" t="s">
         <v>30</v>
       </c>
-      <c r="F3">
-        <v>5</v>
-      </c>
-      <c r="G3">
+      <c r="F3" s="3">
+        <v>5</v>
+      </c>
+      <c r="G3" s="3">
         <v>1</v>
       </c>
       <c r="H3" s="2" t="s">
@@ -798,10 +813,10 @@
       <c r="E4" t="s">
         <v>55</v>
       </c>
-      <c r="F4">
-        <v>5</v>
-      </c>
-      <c r="G4">
+      <c r="F4" s="3">
+        <v>5</v>
+      </c>
+      <c r="G4" s="3">
         <v>1</v>
       </c>
       <c r="H4" s="2" t="s">
@@ -815,10 +830,10 @@
       <c r="E5" t="s">
         <v>69</v>
       </c>
-      <c r="F5">
-        <v>5</v>
-      </c>
-      <c r="G5">
+      <c r="F5" s="3">
+        <v>5</v>
+      </c>
+      <c r="G5" s="3">
         <v>1</v>
       </c>
       <c r="H5" s="2" t="s">
@@ -832,10 +847,10 @@
       <c r="E6" t="s">
         <v>58</v>
       </c>
-      <c r="F6">
-        <v>5</v>
-      </c>
-      <c r="G6">
+      <c r="F6" s="3">
+        <v>5</v>
+      </c>
+      <c r="G6" s="3">
         <v>1</v>
       </c>
       <c r="H6" s="2" t="s">
@@ -849,10 +864,10 @@
       <c r="E7" t="s">
         <v>31</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="3">
         <v>1</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="3">
         <v>1</v>
       </c>
     </row>
@@ -866,10 +881,10 @@
       <c r="E10" t="s">
         <v>49</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="3">
         <v>1</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="3">
         <v>3</v>
       </c>
       <c r="H10" s="2" t="s">
@@ -886,10 +901,10 @@
       <c r="E11" t="s">
         <v>51</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="3">
         <v>2</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="3">
         <v>3</v>
       </c>
       <c r="H11" s="2" t="s">
@@ -906,10 +921,10 @@
       <c r="E12" t="s">
         <v>52</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="3">
         <v>3</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="3">
         <v>3</v>
       </c>
       <c r="H12" s="2" t="s">
@@ -926,58 +941,58 @@
       <c r="E13" t="s">
         <v>46</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="3">
         <v>1</v>
       </c>
-      <c r="G13">
+      <c r="G13" s="3">
         <v>2</v>
       </c>
       <c r="H13" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.45">
-      <c r="C15" t="s">
+    <row r="14" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="D14" t="s">
+        <v>53</v>
+      </c>
+      <c r="E14" t="s">
+        <v>44</v>
+      </c>
+      <c r="F14" s="3">
+        <v>2</v>
+      </c>
+      <c r="G14" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="C16" t="s">
         <v>14</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D16" t="s">
         <v>24</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E16" t="s">
         <v>43</v>
       </c>
-      <c r="F15">
+      <c r="F16" s="3">
         <v>1</v>
       </c>
-      <c r="G15" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.45">
-      <c r="D16" t="s">
-        <v>25</v>
-      </c>
-      <c r="E16" t="s">
-        <v>42</v>
-      </c>
-      <c r="F16">
-        <v>1</v>
-      </c>
-      <c r="G16" t="s">
+      <c r="G16" s="3" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="17" spans="3:8" x14ac:dyDescent="0.45">
       <c r="D17" t="s">
-        <v>53</v>
+        <v>25</v>
       </c>
       <c r="E17" t="s">
-        <v>44</v>
-      </c>
-      <c r="F17">
+        <v>42</v>
+      </c>
+      <c r="F17" s="3">
         <v>1</v>
       </c>
-      <c r="G17" t="s">
+      <c r="G17" s="3" t="s">
         <v>41</v>
       </c>
     </row>
@@ -985,16 +1000,16 @@
       <c r="C19" t="s">
         <v>15</v>
       </c>
-      <c r="D19" s="3" t="s">
+      <c r="D19" s="4" t="s">
         <v>26</v>
       </c>
       <c r="E19" t="s">
         <v>59</v>
       </c>
-      <c r="F19">
-        <v>5</v>
-      </c>
-      <c r="G19">
+      <c r="F19" s="3">
+        <v>5</v>
+      </c>
+      <c r="G19" s="3">
         <v>4</v>
       </c>
       <c r="H19" s="2" t="s">
@@ -1002,11 +1017,11 @@
       </c>
     </row>
     <row r="20" spans="3:8" x14ac:dyDescent="0.45">
-      <c r="D20" s="3"/>
+      <c r="D20" s="4"/>
       <c r="E20" t="s">
         <v>61</v>
       </c>
-      <c r="F20">
+      <c r="F20" s="3">
         <v>5</v>
       </c>
       <c r="H20" s="2" t="s">
@@ -1014,40 +1029,58 @@
       </c>
     </row>
     <row r="21" spans="3:8" x14ac:dyDescent="0.45">
-      <c r="D21" s="3"/>
+      <c r="D21" s="4"/>
       <c r="E21" t="s">
         <v>60</v>
       </c>
-      <c r="F21">
+      <c r="F21" s="3">
         <v>5</v>
       </c>
       <c r="H21" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="22" spans="3:8" ht="34" x14ac:dyDescent="0.45">
-      <c r="D22" s="3" t="s">
+    <row r="22" spans="3:8" x14ac:dyDescent="0.45">
+      <c r="D22" s="4"/>
+      <c r="E22" t="s">
+        <v>75</v>
+      </c>
+      <c r="F22" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="3:8" x14ac:dyDescent="0.45">
+      <c r="D23" s="4"/>
+      <c r="E23" t="s">
+        <v>76</v>
+      </c>
+      <c r="F23" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="3:8" ht="34" x14ac:dyDescent="0.45">
+      <c r="D24" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="E22" s="1" t="s">
+      <c r="E24" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="F22">
-        <v>5</v>
-      </c>
-      <c r="H22" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="23" spans="3:8" x14ac:dyDescent="0.45">
-      <c r="D23" s="3"/>
-      <c r="E23" t="s">
+      <c r="F24" s="3">
+        <v>5</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="25" spans="3:8" x14ac:dyDescent="0.45">
+      <c r="D25" s="4"/>
+      <c r="E25" t="s">
         <v>63</v>
       </c>
-      <c r="F23">
-        <v>5</v>
-      </c>
-      <c r="H23" s="2" t="s">
+      <c r="F25" s="3">
+        <v>5</v>
+      </c>
+      <c r="H25" s="2" t="s">
         <v>47</v>
       </c>
     </row>
@@ -1061,10 +1094,10 @@
       <c r="E27" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F27">
+      <c r="F27" s="3">
         <v>2</v>
       </c>
-      <c r="G27">
+      <c r="G27" s="3">
         <v>2</v>
       </c>
       <c r="H27" s="2" t="s">
@@ -1078,10 +1111,10 @@
       <c r="D29" t="s">
         <v>33</v>
       </c>
-      <c r="F29">
-        <v>5</v>
-      </c>
-      <c r="G29">
+      <c r="F29" s="3">
+        <v>5</v>
+      </c>
+      <c r="G29" s="3">
         <v>3</v>
       </c>
       <c r="H29" s="2" t="s">
@@ -1092,10 +1125,10 @@
       <c r="D30" t="s">
         <v>34</v>
       </c>
-      <c r="F30">
-        <v>5</v>
-      </c>
-      <c r="G30">
+      <c r="F30" s="3">
+        <v>5</v>
+      </c>
+      <c r="G30" s="3">
         <v>3</v>
       </c>
       <c r="H30" s="2" t="s">
@@ -1112,7 +1145,7 @@
       <c r="E34" t="s">
         <v>38</v>
       </c>
-      <c r="F34">
+      <c r="F34" s="3">
         <v>0</v>
       </c>
     </row>
@@ -1126,7 +1159,7 @@
       <c r="E35" t="s">
         <v>38</v>
       </c>
-      <c r="F35">
+      <c r="F35" s="3">
         <v>0</v>
       </c>
       <c r="I35" s="1" t="s">
@@ -1143,7 +1176,7 @@
       <c r="E36" t="s">
         <v>37</v>
       </c>
-      <c r="F36">
+      <c r="F36" s="3">
         <v>0</v>
       </c>
     </row>
@@ -1162,8 +1195,8 @@
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="D19:D21"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="D19:D23"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
[fix bug] a warning window that says plan folder is not existing
</commit_message>
<xml_diff>
--- a/JAM editor요구사항.xlsx
+++ b/JAM editor요구사항.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://o365uos-my.sharepoint.com/personal/2016440063_office_uos_ac_kr/Documents/JAVA/kr.ac.uos.ai.editor.jamEditor/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="55" documentId="13_ncr:1_{E5734DD0-2FF4-40B2-B1BE-1BDDE0E42430}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8D8692FC-4C1D-482D-94E8-AEA1DCD508AA}"/>
+  <xr:revisionPtr revIDLastSave="60" documentId="13_ncr:1_{E5734DD0-2FF4-40B2-B1BE-1BDDE0E42430}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E0AF34A0-EA29-4BDE-B3E5-32574F689F46}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="50" yWindow="40" windowWidth="14580" windowHeight="17900" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="82">
   <si>
     <t>유즈케이스</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -337,6 +337,23 @@
   </si>
   <si>
     <t>run time</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>버그</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>System.out.print가 아닌
+System.our.print도 Coloring을 해버림</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>존재하는 jam파일 삭제하니 플랜 id를 찾을 수 없다는 에러 발생</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>plan 폴더가 없는 프로젝트 열면 plan 폴더가 없다는 에러 발생</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -730,10 +747,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1ABE5394-59B4-47FD-BA35-BF7A817F817E}">
-  <dimension ref="B1:I48"/>
+  <dimension ref="B1:I53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="D53" sqref="D53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -1202,6 +1219,24 @@
         <v>68</v>
       </c>
     </row>
+    <row r="51" spans="3:4" ht="34" x14ac:dyDescent="0.45">
+      <c r="C51" t="s">
+        <v>78</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="52" spans="3:4" x14ac:dyDescent="0.45">
+      <c r="D52" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="53" spans="3:4" x14ac:dyDescent="0.45">
+      <c r="D53" t="s">
+        <v>81</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="D24:D25"/>

</xml_diff>